<commit_message>
end markların gösterilirken ve export edilirken silinmesi, sablonlarin uzerine end markların eklenmesi
</commit_message>
<xml_diff>
--- a/WebApplication1/Forms/01_AylıkDGKrank.xlsx
+++ b/WebApplication1/Forms/01_AylıkDGKrank.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="218">
   <si>
     <t>Skavenc hava sicaklığı ('C) maximum</t>
   </si>
@@ -1167,6 +1167,9 @@
   <si>
     <t>Geminin orijinal alarm sisteminde alarmlar veriyor mu? (Her D/G için bir alarmı test ediniz).</t>
   </si>
+  <si>
+    <t>{END}</t>
+  </si>
 </sst>
 </file>
 
@@ -1175,12 +1178,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2020,20 +2031,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2043,6 +2051,9 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2052,396 +2063,399 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="11" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="6"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="6"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="24" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="24" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="25" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="34" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="34" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="36" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="35" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="35" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4074,7 +4088,7 @@
   <dimension ref="A1:J79"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4092,97 +4106,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="89"/>
-      <c r="B1" s="90"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
+      <c r="A1" s="82"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
     </row>
     <row r="2" spans="1:10" s="39" customFormat="1" ht="56.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="91"/>
-      <c r="B2" s="92" t="s">
+      <c r="A2" s="84"/>
+      <c r="B2" s="107" t="s">
         <v>215</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="91"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="84"/>
     </row>
     <row r="3" spans="1:10" ht="36.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="89"/>
-      <c r="B3" s="95" t="s">
+      <c r="A3" s="82"/>
+      <c r="B3" s="85" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="44"/>
-      <c r="D3" s="96" t="s">
+      <c r="D3" s="86" t="s">
         <v>214</v>
       </c>
-      <c r="E3" s="128"/>
-      <c r="F3" s="128"/>
-      <c r="G3" s="128"/>
-      <c r="H3" s="128"/>
-      <c r="I3" s="127" t="s">
+      <c r="E3" s="121"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="103" t="s">
         <v>213</v>
       </c>
-      <c r="J3" s="89"/>
+      <c r="J3" s="82"/>
     </row>
     <row r="4" spans="1:10" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="89"/>
-      <c r="B4" s="97" t="s">
+      <c r="A4" s="82"/>
+      <c r="B4" s="113" t="s">
         <v>212</v>
       </c>
-      <c r="C4" s="98" t="s">
+      <c r="C4" s="115" t="s">
         <v>211</v>
       </c>
-      <c r="D4" s="99" t="s">
+      <c r="D4" s="117" t="s">
         <v>112</v>
       </c>
-      <c r="E4" s="100" t="s">
+      <c r="E4" s="110" t="s">
         <v>209</v>
       </c>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="103" t="s">
+      <c r="F4" s="111"/>
+      <c r="G4" s="111"/>
+      <c r="H4" s="112"/>
+      <c r="I4" s="119" t="s">
         <v>210</v>
       </c>
-      <c r="J4" s="89"/>
+      <c r="J4" s="82"/>
     </row>
     <row r="5" spans="1:10" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="89"/>
-      <c r="B5" s="104"/>
-      <c r="C5" s="105"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="107" t="s">
+      <c r="A5" s="82"/>
+      <c r="B5" s="114"/>
+      <c r="C5" s="116"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="87" t="s">
         <v>205</v>
       </c>
-      <c r="F5" s="108" t="s">
+      <c r="F5" s="88" t="s">
         <v>206</v>
       </c>
-      <c r="G5" s="108" t="s">
+      <c r="G5" s="88" t="s">
         <v>207</v>
       </c>
-      <c r="H5" s="109" t="s">
+      <c r="H5" s="89" t="s">
         <v>208</v>
       </c>
-      <c r="I5" s="110"/>
-      <c r="J5" s="89"/>
+      <c r="I5" s="120"/>
+      <c r="J5" s="82"/>
     </row>
     <row r="6" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="89"/>
-      <c r="B6" s="111">
+      <c r="A6" s="82"/>
+      <c r="B6" s="90">
         <v>1</v>
       </c>
-      <c r="C6" s="112" t="s">
+      <c r="C6" s="91" t="s">
         <v>113</v>
       </c>
       <c r="D6" s="45"/>
@@ -4191,14 +4205,14 @@
       <c r="G6" s="47"/>
       <c r="H6" s="48"/>
       <c r="I6" s="49"/>
-      <c r="J6" s="89"/>
+      <c r="J6" s="82"/>
     </row>
     <row r="7" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="89"/>
-      <c r="B7" s="113">
+      <c r="A7" s="82"/>
+      <c r="B7" s="92">
         <v>2</v>
       </c>
-      <c r="C7" s="112" t="s">
+      <c r="C7" s="91" t="s">
         <v>114</v>
       </c>
       <c r="D7" s="45"/>
@@ -4207,14 +4221,14 @@
       <c r="G7" s="51"/>
       <c r="H7" s="52"/>
       <c r="I7" s="53"/>
-      <c r="J7" s="89"/>
+      <c r="J7" s="82"/>
     </row>
     <row r="8" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="89"/>
-      <c r="B8" s="113">
+      <c r="A8" s="82"/>
+      <c r="B8" s="92">
         <v>3</v>
       </c>
-      <c r="C8" s="112" t="s">
+      <c r="C8" s="91" t="s">
         <v>167</v>
       </c>
       <c r="D8" s="45"/>
@@ -4223,14 +4237,14 @@
       <c r="G8" s="51"/>
       <c r="H8" s="52"/>
       <c r="I8" s="53"/>
-      <c r="J8" s="89"/>
+      <c r="J8" s="82"/>
     </row>
     <row r="9" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="89"/>
-      <c r="B9" s="113">
+      <c r="A9" s="82"/>
+      <c r="B9" s="92">
         <v>4</v>
       </c>
-      <c r="C9" s="112" t="s">
+      <c r="C9" s="91" t="s">
         <v>183</v>
       </c>
       <c r="D9" s="45"/>
@@ -4239,14 +4253,14 @@
       <c r="G9" s="51"/>
       <c r="H9" s="52"/>
       <c r="I9" s="53"/>
-      <c r="J9" s="89"/>
+      <c r="J9" s="82"/>
     </row>
     <row r="10" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="89"/>
-      <c r="B10" s="113">
+      <c r="A10" s="82"/>
+      <c r="B10" s="92">
         <v>5</v>
       </c>
-      <c r="C10" s="112" t="s">
+      <c r="C10" s="91" t="s">
         <v>184</v>
       </c>
       <c r="D10" s="45"/>
@@ -4255,14 +4269,14 @@
       <c r="G10" s="51"/>
       <c r="H10" s="52"/>
       <c r="I10" s="53"/>
-      <c r="J10" s="89"/>
+      <c r="J10" s="82"/>
     </row>
     <row r="11" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="89"/>
-      <c r="B11" s="113">
+      <c r="A11" s="82"/>
+      <c r="B11" s="92">
         <v>6</v>
       </c>
-      <c r="C11" s="114" t="s">
+      <c r="C11" s="93" t="s">
         <v>115</v>
       </c>
       <c r="D11" s="45"/>
@@ -4271,14 +4285,14 @@
       <c r="G11" s="51"/>
       <c r="H11" s="52"/>
       <c r="I11" s="53"/>
-      <c r="J11" s="89"/>
+      <c r="J11" s="82"/>
     </row>
     <row r="12" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="89"/>
-      <c r="B12" s="113">
+      <c r="A12" s="82"/>
+      <c r="B12" s="92">
         <v>7</v>
       </c>
-      <c r="C12" s="114" t="s">
+      <c r="C12" s="93" t="s">
         <v>116</v>
       </c>
       <c r="D12" s="45"/>
@@ -4287,14 +4301,14 @@
       <c r="G12" s="51"/>
       <c r="H12" s="52"/>
       <c r="I12" s="53"/>
-      <c r="J12" s="89"/>
+      <c r="J12" s="82"/>
     </row>
     <row r="13" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="89"/>
-      <c r="B13" s="113">
+      <c r="A13" s="82"/>
+      <c r="B13" s="92">
         <v>8</v>
       </c>
-      <c r="C13" s="114" t="s">
+      <c r="C13" s="93" t="s">
         <v>117</v>
       </c>
       <c r="D13" s="54"/>
@@ -4303,14 +4317,14 @@
       <c r="G13" s="56"/>
       <c r="H13" s="57"/>
       <c r="I13" s="58"/>
-      <c r="J13" s="89"/>
+      <c r="J13" s="82"/>
     </row>
     <row r="14" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="89"/>
-      <c r="B14" s="113">
+      <c r="A14" s="82"/>
+      <c r="B14" s="92">
         <v>9</v>
       </c>
-      <c r="C14" s="114" t="s">
+      <c r="C14" s="93" t="s">
         <v>118</v>
       </c>
       <c r="D14" s="54"/>
@@ -4319,14 +4333,14 @@
       <c r="G14" s="56"/>
       <c r="H14" s="57"/>
       <c r="I14" s="58"/>
-      <c r="J14" s="89"/>
+      <c r="J14" s="82"/>
     </row>
     <row r="15" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="89"/>
-      <c r="B15" s="113">
+      <c r="A15" s="82"/>
+      <c r="B15" s="92">
         <v>10</v>
       </c>
-      <c r="C15" s="114" t="s">
+      <c r="C15" s="93" t="s">
         <v>119</v>
       </c>
       <c r="D15" s="54"/>
@@ -4335,14 +4349,14 @@
       <c r="G15" s="56"/>
       <c r="H15" s="57"/>
       <c r="I15" s="58"/>
-      <c r="J15" s="89"/>
+      <c r="J15" s="82"/>
     </row>
     <row r="16" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="89"/>
-      <c r="B16" s="113">
+      <c r="A16" s="82"/>
+      <c r="B16" s="92">
         <v>11</v>
       </c>
-      <c r="C16" s="114" t="s">
+      <c r="C16" s="93" t="s">
         <v>166</v>
       </c>
       <c r="D16" s="54"/>
@@ -4351,14 +4365,14 @@
       <c r="G16" s="56"/>
       <c r="H16" s="57"/>
       <c r="I16" s="58"/>
-      <c r="J16" s="89"/>
+      <c r="J16" s="82"/>
     </row>
     <row r="17" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="89"/>
-      <c r="B17" s="113">
+      <c r="A17" s="82"/>
+      <c r="B17" s="92">
         <v>12</v>
       </c>
-      <c r="C17" s="114" t="s">
+      <c r="C17" s="93" t="s">
         <v>168</v>
       </c>
       <c r="D17" s="59"/>
@@ -4367,14 +4381,14 @@
       <c r="G17" s="56"/>
       <c r="H17" s="57"/>
       <c r="I17" s="58"/>
-      <c r="J17" s="89"/>
+      <c r="J17" s="82"/>
     </row>
     <row r="18" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="89"/>
-      <c r="B18" s="113">
+      <c r="A18" s="82"/>
+      <c r="B18" s="92">
         <v>13</v>
       </c>
-      <c r="C18" s="114" t="s">
+      <c r="C18" s="93" t="s">
         <v>176</v>
       </c>
       <c r="D18" s="60"/>
@@ -4383,14 +4397,14 @@
       <c r="G18" s="56"/>
       <c r="H18" s="57"/>
       <c r="I18" s="58"/>
-      <c r="J18" s="89"/>
+      <c r="J18" s="82"/>
     </row>
     <row r="19" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="89"/>
-      <c r="B19" s="113">
+      <c r="A19" s="82"/>
+      <c r="B19" s="92">
         <v>14</v>
       </c>
-      <c r="C19" s="114" t="s">
+      <c r="C19" s="93" t="s">
         <v>120</v>
       </c>
       <c r="D19" s="60"/>
@@ -4399,14 +4413,14 @@
       <c r="G19" s="56"/>
       <c r="H19" s="57"/>
       <c r="I19" s="58"/>
-      <c r="J19" s="89"/>
+      <c r="J19" s="82"/>
     </row>
     <row r="20" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="89"/>
-      <c r="B20" s="113">
+      <c r="A20" s="82"/>
+      <c r="B20" s="92">
         <v>15</v>
       </c>
-      <c r="C20" s="114" t="s">
+      <c r="C20" s="93" t="s">
         <v>121</v>
       </c>
       <c r="D20" s="60"/>
@@ -4415,14 +4429,14 @@
       <c r="G20" s="56"/>
       <c r="H20" s="57"/>
       <c r="I20" s="58"/>
-      <c r="J20" s="89"/>
+      <c r="J20" s="82"/>
     </row>
     <row r="21" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="89"/>
-      <c r="B21" s="113">
+      <c r="A21" s="82"/>
+      <c r="B21" s="92">
         <v>16</v>
       </c>
-      <c r="C21" s="114" t="s">
+      <c r="C21" s="93" t="s">
         <v>109</v>
       </c>
       <c r="D21" s="59"/>
@@ -4431,14 +4445,14 @@
       <c r="G21" s="56"/>
       <c r="H21" s="57"/>
       <c r="I21" s="58"/>
-      <c r="J21" s="89"/>
+      <c r="J21" s="82"/>
     </row>
     <row r="22" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="89"/>
-      <c r="B22" s="113">
+      <c r="A22" s="82"/>
+      <c r="B22" s="92">
         <v>17</v>
       </c>
-      <c r="C22" s="114" t="s">
+      <c r="C22" s="93" t="s">
         <v>110</v>
       </c>
       <c r="D22" s="59"/>
@@ -4447,14 +4461,14 @@
       <c r="G22" s="56"/>
       <c r="H22" s="57"/>
       <c r="I22" s="58"/>
-      <c r="J22" s="89"/>
+      <c r="J22" s="82"/>
     </row>
     <row r="23" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="89"/>
-      <c r="B23" s="113">
+      <c r="A23" s="82"/>
+      <c r="B23" s="92">
         <v>18</v>
       </c>
-      <c r="C23" s="114" t="s">
+      <c r="C23" s="93" t="s">
         <v>122</v>
       </c>
       <c r="D23" s="59"/>
@@ -4463,14 +4477,14 @@
       <c r="G23" s="56"/>
       <c r="H23" s="57"/>
       <c r="I23" s="58"/>
-      <c r="J23" s="89"/>
+      <c r="J23" s="82"/>
     </row>
     <row r="24" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="89"/>
-      <c r="B24" s="113">
+      <c r="A24" s="82"/>
+      <c r="B24" s="92">
         <v>19</v>
       </c>
-      <c r="C24" s="114" t="s">
+      <c r="C24" s="93" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="59"/>
@@ -4479,14 +4493,14 @@
       <c r="G24" s="56"/>
       <c r="H24" s="57"/>
       <c r="I24" s="58"/>
-      <c r="J24" s="89"/>
+      <c r="J24" s="82"/>
     </row>
     <row r="25" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="89"/>
-      <c r="B25" s="113">
+      <c r="A25" s="82"/>
+      <c r="B25" s="92">
         <v>20</v>
       </c>
-      <c r="C25" s="114" t="s">
+      <c r="C25" s="93" t="s">
         <v>177</v>
       </c>
       <c r="D25" s="60"/>
@@ -4495,14 +4509,14 @@
       <c r="G25" s="56"/>
       <c r="H25" s="57"/>
       <c r="I25" s="58"/>
-      <c r="J25" s="89"/>
+      <c r="J25" s="82"/>
     </row>
     <row r="26" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="89"/>
-      <c r="B26" s="113">
+      <c r="A26" s="82"/>
+      <c r="B26" s="92">
         <v>21</v>
       </c>
-      <c r="C26" s="114" t="s">
+      <c r="C26" s="93" t="s">
         <v>2</v>
       </c>
       <c r="D26" s="60"/>
@@ -4511,14 +4525,14 @@
       <c r="G26" s="56"/>
       <c r="H26" s="57"/>
       <c r="I26" s="58"/>
-      <c r="J26" s="89"/>
+      <c r="J26" s="82"/>
     </row>
     <row r="27" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="89"/>
-      <c r="B27" s="113">
+      <c r="A27" s="82"/>
+      <c r="B27" s="92">
         <v>22</v>
       </c>
-      <c r="C27" s="114" t="s">
+      <c r="C27" s="93" t="s">
         <v>123</v>
       </c>
       <c r="D27" s="60"/>
@@ -4527,14 +4541,14 @@
       <c r="G27" s="56"/>
       <c r="H27" s="57"/>
       <c r="I27" s="58"/>
-      <c r="J27" s="89"/>
+      <c r="J27" s="82"/>
     </row>
     <row r="28" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="89"/>
-      <c r="B28" s="113">
+      <c r="A28" s="82"/>
+      <c r="B28" s="92">
         <v>23</v>
       </c>
-      <c r="C28" s="114" t="s">
+      <c r="C28" s="93" t="s">
         <v>124</v>
       </c>
       <c r="D28" s="60"/>
@@ -4543,14 +4557,14 @@
       <c r="G28" s="56"/>
       <c r="H28" s="57"/>
       <c r="I28" s="58"/>
-      <c r="J28" s="89"/>
+      <c r="J28" s="82"/>
     </row>
     <row r="29" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="89"/>
-      <c r="B29" s="113">
+      <c r="A29" s="82"/>
+      <c r="B29" s="92">
         <v>24</v>
       </c>
-      <c r="C29" s="114" t="s">
+      <c r="C29" s="93" t="s">
         <v>125</v>
       </c>
       <c r="D29" s="60"/>
@@ -4559,14 +4573,14 @@
       <c r="G29" s="56"/>
       <c r="H29" s="57"/>
       <c r="I29" s="58"/>
-      <c r="J29" s="89"/>
+      <c r="J29" s="82"/>
     </row>
     <row r="30" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="89"/>
-      <c r="B30" s="113">
+      <c r="A30" s="82"/>
+      <c r="B30" s="92">
         <v>25</v>
       </c>
-      <c r="C30" s="114" t="s">
+      <c r="C30" s="93" t="s">
         <v>126</v>
       </c>
       <c r="D30" s="60"/>
@@ -4575,14 +4589,14 @@
       <c r="G30" s="56"/>
       <c r="H30" s="57"/>
       <c r="I30" s="58"/>
-      <c r="J30" s="89"/>
+      <c r="J30" s="82"/>
     </row>
     <row r="31" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="89"/>
-      <c r="B31" s="113">
+      <c r="A31" s="82"/>
+      <c r="B31" s="92">
         <v>26</v>
       </c>
-      <c r="C31" s="114" t="s">
+      <c r="C31" s="93" t="s">
         <v>127</v>
       </c>
       <c r="D31" s="60"/>
@@ -4591,14 +4605,14 @@
       <c r="G31" s="56"/>
       <c r="H31" s="57"/>
       <c r="I31" s="58"/>
-      <c r="J31" s="89"/>
+      <c r="J31" s="82"/>
     </row>
     <row r="32" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="89"/>
-      <c r="B32" s="113">
+      <c r="A32" s="82"/>
+      <c r="B32" s="92">
         <v>27</v>
       </c>
-      <c r="C32" s="114" t="s">
+      <c r="C32" s="93" t="s">
         <v>128</v>
       </c>
       <c r="D32" s="60"/>
@@ -4607,14 +4621,14 @@
       <c r="G32" s="56"/>
       <c r="H32" s="57"/>
       <c r="I32" s="58"/>
-      <c r="J32" s="89"/>
+      <c r="J32" s="82"/>
     </row>
     <row r="33" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="89"/>
-      <c r="B33" s="113">
+      <c r="A33" s="82"/>
+      <c r="B33" s="92">
         <v>28</v>
       </c>
-      <c r="C33" s="114" t="s">
+      <c r="C33" s="93" t="s">
         <v>204</v>
       </c>
       <c r="D33" s="60"/>
@@ -4623,14 +4637,14 @@
       <c r="G33" s="56"/>
       <c r="H33" s="57"/>
       <c r="I33" s="58"/>
-      <c r="J33" s="89"/>
+      <c r="J33" s="82"/>
     </row>
     <row r="34" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="89"/>
-      <c r="B34" s="113">
+      <c r="A34" s="82"/>
+      <c r="B34" s="92">
         <v>29</v>
       </c>
-      <c r="C34" s="114" t="s">
+      <c r="C34" s="93" t="s">
         <v>129</v>
       </c>
       <c r="D34" s="60"/>
@@ -4639,14 +4653,14 @@
       <c r="G34" s="56"/>
       <c r="H34" s="57"/>
       <c r="I34" s="58"/>
-      <c r="J34" s="89"/>
+      <c r="J34" s="82"/>
     </row>
     <row r="35" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="89"/>
-      <c r="B35" s="113">
+      <c r="A35" s="82"/>
+      <c r="B35" s="92">
         <v>30</v>
       </c>
-      <c r="C35" s="114" t="s">
+      <c r="C35" s="93" t="s">
         <v>130</v>
       </c>
       <c r="D35" s="60"/>
@@ -4655,14 +4669,14 @@
       <c r="G35" s="56"/>
       <c r="H35" s="57"/>
       <c r="I35" s="58"/>
-      <c r="J35" s="89"/>
+      <c r="J35" s="82"/>
     </row>
     <row r="36" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="89"/>
-      <c r="B36" s="113">
+      <c r="A36" s="82"/>
+      <c r="B36" s="92">
         <v>31</v>
       </c>
-      <c r="C36" s="114" t="s">
+      <c r="C36" s="93" t="s">
         <v>131</v>
       </c>
       <c r="D36" s="60"/>
@@ -4671,14 +4685,14 @@
       <c r="G36" s="56"/>
       <c r="H36" s="57"/>
       <c r="I36" s="58"/>
-      <c r="J36" s="89"/>
+      <c r="J36" s="82"/>
     </row>
     <row r="37" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="89"/>
-      <c r="B37" s="113">
+      <c r="A37" s="82"/>
+      <c r="B37" s="92">
         <v>32</v>
       </c>
-      <c r="C37" s="114" t="s">
+      <c r="C37" s="93" t="s">
         <v>132</v>
       </c>
       <c r="D37" s="60"/>
@@ -4687,14 +4701,14 @@
       <c r="G37" s="56"/>
       <c r="H37" s="57"/>
       <c r="I37" s="58"/>
-      <c r="J37" s="89"/>
+      <c r="J37" s="82"/>
     </row>
     <row r="38" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="89"/>
-      <c r="B38" s="113">
+      <c r="A38" s="82"/>
+      <c r="B38" s="92">
         <v>33</v>
       </c>
-      <c r="C38" s="114" t="s">
+      <c r="C38" s="93" t="s">
         <v>133</v>
       </c>
       <c r="D38" s="60"/>
@@ -4703,14 +4717,14 @@
       <c r="G38" s="56"/>
       <c r="H38" s="57"/>
       <c r="I38" s="58"/>
-      <c r="J38" s="89"/>
+      <c r="J38" s="82"/>
     </row>
     <row r="39" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="89"/>
-      <c r="B39" s="113">
+      <c r="A39" s="82"/>
+      <c r="B39" s="92">
         <v>34</v>
       </c>
-      <c r="C39" s="114" t="s">
+      <c r="C39" s="93" t="s">
         <v>134</v>
       </c>
       <c r="D39" s="60"/>
@@ -4719,14 +4733,14 @@
       <c r="G39" s="56"/>
       <c r="H39" s="57"/>
       <c r="I39" s="58"/>
-      <c r="J39" s="89"/>
+      <c r="J39" s="82"/>
     </row>
     <row r="40" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="89"/>
-      <c r="B40" s="113">
+      <c r="A40" s="82"/>
+      <c r="B40" s="92">
         <v>35</v>
       </c>
-      <c r="C40" s="114" t="s">
+      <c r="C40" s="93" t="s">
         <v>135</v>
       </c>
       <c r="D40" s="60"/>
@@ -4735,14 +4749,14 @@
       <c r="G40" s="56"/>
       <c r="H40" s="57"/>
       <c r="I40" s="58"/>
-      <c r="J40" s="89"/>
+      <c r="J40" s="82"/>
     </row>
     <row r="41" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="89"/>
-      <c r="B41" s="113">
+      <c r="A41" s="82"/>
+      <c r="B41" s="92">
         <v>36</v>
       </c>
-      <c r="C41" s="114" t="s">
+      <c r="C41" s="93" t="s">
         <v>136</v>
       </c>
       <c r="D41" s="60"/>
@@ -4751,14 +4765,14 @@
       <c r="G41" s="56"/>
       <c r="H41" s="57"/>
       <c r="I41" s="58"/>
-      <c r="J41" s="89"/>
+      <c r="J41" s="82"/>
     </row>
     <row r="42" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="89"/>
-      <c r="B42" s="113">
-        <v>37</v>
-      </c>
-      <c r="C42" s="114" t="s">
+      <c r="A42" s="82"/>
+      <c r="B42" s="92">
+        <v>37</v>
+      </c>
+      <c r="C42" s="93" t="s">
         <v>169</v>
       </c>
       <c r="D42" s="60"/>
@@ -4767,14 +4781,14 @@
       <c r="G42" s="56"/>
       <c r="H42" s="57"/>
       <c r="I42" s="58"/>
-      <c r="J42" s="89"/>
+      <c r="J42" s="82"/>
     </row>
     <row r="43" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="89"/>
-      <c r="B43" s="113">
+      <c r="A43" s="82"/>
+      <c r="B43" s="92">
         <v>38</v>
       </c>
-      <c r="C43" s="114" t="s">
+      <c r="C43" s="93" t="s">
         <v>171</v>
       </c>
       <c r="D43" s="60"/>
@@ -4783,14 +4797,14 @@
       <c r="G43" s="56"/>
       <c r="H43" s="57"/>
       <c r="I43" s="58"/>
-      <c r="J43" s="89"/>
+      <c r="J43" s="82"/>
     </row>
     <row r="44" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="89"/>
-      <c r="B44" s="113">
+      <c r="A44" s="82"/>
+      <c r="B44" s="92">
         <v>39</v>
       </c>
-      <c r="C44" s="114" t="s">
+      <c r="C44" s="93" t="s">
         <v>111</v>
       </c>
       <c r="D44" s="60"/>
@@ -4799,14 +4813,14 @@
       <c r="G44" s="56"/>
       <c r="H44" s="57"/>
       <c r="I44" s="58"/>
-      <c r="J44" s="89"/>
+      <c r="J44" s="82"/>
     </row>
     <row r="45" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="89"/>
-      <c r="B45" s="113">
+      <c r="A45" s="82"/>
+      <c r="B45" s="92">
         <v>40</v>
       </c>
-      <c r="C45" s="114" t="s">
+      <c r="C45" s="93" t="s">
         <v>137</v>
       </c>
       <c r="D45" s="60"/>
@@ -4815,14 +4829,14 @@
       <c r="G45" s="56"/>
       <c r="H45" s="57"/>
       <c r="I45" s="58"/>
-      <c r="J45" s="89"/>
+      <c r="J45" s="82"/>
     </row>
     <row r="46" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="89"/>
-      <c r="B46" s="113">
+      <c r="A46" s="82"/>
+      <c r="B46" s="92">
         <v>41</v>
       </c>
-      <c r="C46" s="114" t="s">
+      <c r="C46" s="93" t="s">
         <v>170</v>
       </c>
       <c r="D46" s="60"/>
@@ -4831,14 +4845,14 @@
       <c r="G46" s="56"/>
       <c r="H46" s="57"/>
       <c r="I46" s="58"/>
-      <c r="J46" s="89"/>
+      <c r="J46" s="82"/>
     </row>
     <row r="47" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="89"/>
-      <c r="B47" s="113">
+      <c r="A47" s="82"/>
+      <c r="B47" s="92">
         <v>42</v>
       </c>
-      <c r="C47" s="114" t="s">
+      <c r="C47" s="93" t="s">
         <v>138</v>
       </c>
       <c r="D47" s="60"/>
@@ -4847,14 +4861,14 @@
       <c r="G47" s="56"/>
       <c r="H47" s="57"/>
       <c r="I47" s="58"/>
-      <c r="J47" s="89"/>
+      <c r="J47" s="82"/>
     </row>
     <row r="48" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="89"/>
-      <c r="B48" s="113">
+      <c r="A48" s="82"/>
+      <c r="B48" s="92">
         <v>43</v>
       </c>
-      <c r="C48" s="115" t="s">
+      <c r="C48" s="94" t="s">
         <v>139</v>
       </c>
       <c r="D48" s="60"/>
@@ -4863,14 +4877,14 @@
       <c r="G48" s="62"/>
       <c r="H48" s="63"/>
       <c r="I48" s="64"/>
-      <c r="J48" s="89"/>
+      <c r="J48" s="82"/>
     </row>
     <row r="49" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="89"/>
-      <c r="B49" s="113">
+      <c r="A49" s="82"/>
+      <c r="B49" s="92">
         <v>44</v>
       </c>
-      <c r="C49" s="114" t="s">
+      <c r="C49" s="93" t="s">
         <v>140</v>
       </c>
       <c r="D49" s="60"/>
@@ -4879,14 +4893,14 @@
       <c r="G49" s="56"/>
       <c r="H49" s="57"/>
       <c r="I49" s="58"/>
-      <c r="J49" s="89"/>
+      <c r="J49" s="82"/>
     </row>
     <row r="50" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="89"/>
-      <c r="B50" s="113">
+      <c r="A50" s="82"/>
+      <c r="B50" s="92">
         <v>45</v>
       </c>
-      <c r="C50" s="114" t="s">
+      <c r="C50" s="93" t="s">
         <v>141</v>
       </c>
       <c r="D50" s="60"/>
@@ -4895,14 +4909,14 @@
       <c r="G50" s="56"/>
       <c r="H50" s="57"/>
       <c r="I50" s="58"/>
-      <c r="J50" s="89"/>
+      <c r="J50" s="82"/>
     </row>
     <row r="51" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="89"/>
-      <c r="B51" s="113">
+      <c r="A51" s="82"/>
+      <c r="B51" s="92">
         <v>46</v>
       </c>
-      <c r="C51" s="115" t="s">
+      <c r="C51" s="94" t="s">
         <v>142</v>
       </c>
       <c r="D51" s="60"/>
@@ -4911,14 +4925,14 @@
       <c r="G51" s="56"/>
       <c r="H51" s="57"/>
       <c r="I51" s="64"/>
-      <c r="J51" s="89"/>
+      <c r="J51" s="82"/>
     </row>
     <row r="52" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="89"/>
-      <c r="B52" s="113">
+      <c r="A52" s="82"/>
+      <c r="B52" s="92">
         <v>47</v>
       </c>
-      <c r="C52" s="115" t="s">
+      <c r="C52" s="94" t="s">
         <v>162</v>
       </c>
       <c r="D52" s="65"/>
@@ -4927,14 +4941,14 @@
       <c r="G52" s="62"/>
       <c r="H52" s="63"/>
       <c r="I52" s="64"/>
-      <c r="J52" s="89"/>
+      <c r="J52" s="82"/>
     </row>
     <row r="53" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="89"/>
-      <c r="B53" s="113">
+      <c r="A53" s="82"/>
+      <c r="B53" s="92">
         <v>48</v>
       </c>
-      <c r="C53" s="112" t="s">
+      <c r="C53" s="91" t="s">
         <v>146</v>
       </c>
       <c r="D53" s="65"/>
@@ -4943,14 +4957,14 @@
       <c r="G53" s="62"/>
       <c r="H53" s="63"/>
       <c r="I53" s="64"/>
-      <c r="J53" s="89"/>
+      <c r="J53" s="82"/>
     </row>
     <row r="54" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="89"/>
-      <c r="B54" s="113">
+      <c r="A54" s="82"/>
+      <c r="B54" s="92">
         <v>49</v>
       </c>
-      <c r="C54" s="112" t="s">
+      <c r="C54" s="91" t="s">
         <v>178</v>
       </c>
       <c r="D54" s="65"/>
@@ -4959,14 +4973,14 @@
       <c r="G54" s="62"/>
       <c r="H54" s="63"/>
       <c r="I54" s="64"/>
-      <c r="J54" s="89"/>
+      <c r="J54" s="82"/>
     </row>
     <row r="55" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="89"/>
-      <c r="B55" s="113">
+      <c r="A55" s="82"/>
+      <c r="B55" s="92">
         <v>50</v>
       </c>
-      <c r="C55" s="112" t="s">
+      <c r="C55" s="91" t="s">
         <v>179</v>
       </c>
       <c r="D55" s="65"/>
@@ -4975,14 +4989,14 @@
       <c r="G55" s="62"/>
       <c r="H55" s="63"/>
       <c r="I55" s="64"/>
-      <c r="J55" s="89"/>
+      <c r="J55" s="82"/>
     </row>
     <row r="56" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="89"/>
-      <c r="B56" s="113">
+      <c r="A56" s="82"/>
+      <c r="B56" s="92">
         <v>51</v>
       </c>
-      <c r="C56" s="112" t="s">
+      <c r="C56" s="91" t="s">
         <v>143</v>
       </c>
       <c r="D56" s="65"/>
@@ -4991,14 +5005,14 @@
       <c r="G56" s="62"/>
       <c r="H56" s="63"/>
       <c r="I56" s="64"/>
-      <c r="J56" s="89"/>
+      <c r="J56" s="82"/>
     </row>
     <row r="57" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="89"/>
-      <c r="B57" s="113">
+      <c r="A57" s="82"/>
+      <c r="B57" s="92">
         <v>52</v>
       </c>
-      <c r="C57" s="112" t="s">
+      <c r="C57" s="91" t="s">
         <v>203</v>
       </c>
       <c r="D57" s="65"/>
@@ -5007,14 +5021,14 @@
       <c r="G57" s="62"/>
       <c r="H57" s="63"/>
       <c r="I57" s="64"/>
-      <c r="J57" s="89"/>
+      <c r="J57" s="82"/>
     </row>
     <row r="58" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="89"/>
-      <c r="B58" s="113">
+      <c r="A58" s="82"/>
+      <c r="B58" s="92">
         <v>53</v>
       </c>
-      <c r="C58" s="112" t="s">
+      <c r="C58" s="91" t="s">
         <v>172</v>
       </c>
       <c r="D58" s="65"/>
@@ -5023,14 +5037,14 @@
       <c r="G58" s="62"/>
       <c r="H58" s="63"/>
       <c r="I58" s="64"/>
-      <c r="J58" s="89"/>
+      <c r="J58" s="82"/>
     </row>
     <row r="59" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="89"/>
-      <c r="B59" s="113">
+      <c r="A59" s="82"/>
+      <c r="B59" s="92">
         <v>54</v>
       </c>
-      <c r="C59" s="112" t="s">
+      <c r="C59" s="91" t="s">
         <v>194</v>
       </c>
       <c r="D59" s="65"/>
@@ -5039,14 +5053,14 @@
       <c r="G59" s="62"/>
       <c r="H59" s="63"/>
       <c r="I59" s="64"/>
-      <c r="J59" s="89"/>
+      <c r="J59" s="82"/>
     </row>
     <row r="60" spans="1:10" ht="93" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="89"/>
-      <c r="B60" s="113">
+      <c r="A60" s="82"/>
+      <c r="B60" s="92">
         <v>55</v>
       </c>
-      <c r="C60" s="116" t="s">
+      <c r="C60" s="95" t="s">
         <v>196</v>
       </c>
       <c r="D60" s="65"/>
@@ -5055,14 +5069,14 @@
       <c r="G60" s="62"/>
       <c r="H60" s="63"/>
       <c r="I60" s="64"/>
-      <c r="J60" s="89"/>
+      <c r="J60" s="82"/>
     </row>
     <row r="61" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="89"/>
-      <c r="B61" s="113">
+      <c r="A61" s="82"/>
+      <c r="B61" s="92">
         <v>56</v>
       </c>
-      <c r="C61" s="117" t="s">
+      <c r="C61" s="96" t="s">
         <v>202</v>
       </c>
       <c r="D61" s="65"/>
@@ -5071,14 +5085,14 @@
       <c r="G61" s="62"/>
       <c r="H61" s="63"/>
       <c r="I61" s="64"/>
-      <c r="J61" s="89"/>
+      <c r="J61" s="82"/>
     </row>
     <row r="62" spans="1:10" ht="132" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="89"/>
-      <c r="B62" s="113">
+      <c r="A62" s="82"/>
+      <c r="B62" s="92">
         <v>57</v>
       </c>
-      <c r="C62" s="114" t="s">
+      <c r="C62" s="93" t="s">
         <v>195</v>
       </c>
       <c r="D62" s="66"/>
@@ -5087,14 +5101,14 @@
       <c r="G62" s="56"/>
       <c r="H62" s="57"/>
       <c r="I62" s="58"/>
-      <c r="J62" s="89"/>
+      <c r="J62" s="82"/>
     </row>
     <row r="63" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="89"/>
-      <c r="B63" s="113">
+      <c r="A63" s="82"/>
+      <c r="B63" s="92">
         <v>58</v>
       </c>
-      <c r="C63" s="114" t="s">
+      <c r="C63" s="93" t="s">
         <v>201</v>
       </c>
       <c r="D63" s="67"/>
@@ -5103,14 +5117,14 @@
       <c r="G63" s="69"/>
       <c r="H63" s="70"/>
       <c r="I63" s="71"/>
-      <c r="J63" s="89"/>
+      <c r="J63" s="82"/>
     </row>
     <row r="64" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="89"/>
-      <c r="B64" s="113">
+      <c r="A64" s="82"/>
+      <c r="B64" s="92">
         <v>59</v>
       </c>
-      <c r="C64" s="116" t="s">
+      <c r="C64" s="95" t="s">
         <v>144</v>
       </c>
       <c r="D64" s="72"/>
@@ -5119,14 +5133,14 @@
       <c r="G64" s="69"/>
       <c r="H64" s="70"/>
       <c r="I64" s="73"/>
-      <c r="J64" s="89"/>
+      <c r="J64" s="82"/>
     </row>
     <row r="65" spans="1:10" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="89"/>
-      <c r="B65" s="113">
+      <c r="A65" s="82"/>
+      <c r="B65" s="92">
         <v>60</v>
       </c>
-      <c r="C65" s="118" t="s">
+      <c r="C65" s="97" t="s">
         <v>145</v>
       </c>
       <c r="D65" s="74"/>
@@ -5135,28 +5149,28 @@
       <c r="G65" s="76"/>
       <c r="H65" s="77"/>
       <c r="I65" s="78"/>
-      <c r="J65" s="89"/>
+      <c r="J65" s="82"/>
     </row>
     <row r="66" spans="1:10" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="89"/>
-      <c r="B66" s="119" t="s">
+      <c r="A66" s="82"/>
+      <c r="B66" s="104" t="s">
         <v>190</v>
       </c>
-      <c r="C66" s="120"/>
-      <c r="D66" s="120"/>
-      <c r="E66" s="120"/>
-      <c r="F66" s="120"/>
-      <c r="G66" s="120"/>
-      <c r="H66" s="120"/>
-      <c r="I66" s="121"/>
-      <c r="J66" s="89"/>
+      <c r="C66" s="105"/>
+      <c r="D66" s="105"/>
+      <c r="E66" s="105"/>
+      <c r="F66" s="105"/>
+      <c r="G66" s="105"/>
+      <c r="H66" s="105"/>
+      <c r="I66" s="106"/>
+      <c r="J66" s="82"/>
     </row>
     <row r="67" spans="1:10" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="89"/>
-      <c r="B67" s="111">
+      <c r="A67" s="82"/>
+      <c r="B67" s="90">
         <v>61</v>
       </c>
-      <c r="C67" s="122" t="s">
+      <c r="C67" s="98" t="s">
         <v>191</v>
       </c>
       <c r="D67" s="79"/>
@@ -5165,14 +5179,14 @@
       <c r="G67" s="80"/>
       <c r="H67" s="80"/>
       <c r="I67" s="81"/>
-      <c r="J67" s="89"/>
+      <c r="J67" s="82"/>
     </row>
     <row r="68" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="89"/>
-      <c r="B68" s="113">
+      <c r="A68" s="82"/>
+      <c r="B68" s="92">
         <v>62</v>
       </c>
-      <c r="C68" s="123" t="s">
+      <c r="C68" s="99" t="s">
         <v>192</v>
       </c>
       <c r="D68" s="56"/>
@@ -5181,14 +5195,14 @@
       <c r="G68" s="56"/>
       <c r="H68" s="56"/>
       <c r="I68" s="57"/>
-      <c r="J68" s="89"/>
+      <c r="J68" s="82"/>
     </row>
     <row r="69" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="89"/>
-      <c r="B69" s="111">
+      <c r="A69" s="82"/>
+      <c r="B69" s="90">
         <v>63</v>
       </c>
-      <c r="C69" s="124" t="s">
+      <c r="C69" s="100" t="s">
         <v>200</v>
       </c>
       <c r="D69" s="56"/>
@@ -5197,14 +5211,14 @@
       <c r="G69" s="56"/>
       <c r="H69" s="56"/>
       <c r="I69" s="57"/>
-      <c r="J69" s="89"/>
+      <c r="J69" s="82"/>
     </row>
     <row r="70" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="89"/>
-      <c r="B70" s="113">
+      <c r="A70" s="82"/>
+      <c r="B70" s="92">
         <v>64</v>
       </c>
-      <c r="C70" s="124" t="s">
+      <c r="C70" s="100" t="s">
         <v>199</v>
       </c>
       <c r="D70" s="56"/>
@@ -5213,14 +5227,14 @@
       <c r="G70" s="56"/>
       <c r="H70" s="56"/>
       <c r="I70" s="57"/>
-      <c r="J70" s="89"/>
+      <c r="J70" s="82"/>
     </row>
     <row r="71" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="89"/>
-      <c r="B71" s="111">
+      <c r="A71" s="82"/>
+      <c r="B71" s="90">
         <v>65</v>
       </c>
-      <c r="C71" s="124" t="s">
+      <c r="C71" s="100" t="s">
         <v>180</v>
       </c>
       <c r="D71" s="56"/>
@@ -5229,14 +5243,14 @@
       <c r="G71" s="56"/>
       <c r="H71" s="56"/>
       <c r="I71" s="57"/>
-      <c r="J71" s="89"/>
+      <c r="J71" s="82"/>
     </row>
     <row r="72" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="89"/>
-      <c r="B72" s="113">
+      <c r="A72" s="82"/>
+      <c r="B72" s="92">
         <v>66</v>
       </c>
-      <c r="C72" s="124" t="s">
+      <c r="C72" s="100" t="s">
         <v>163</v>
       </c>
       <c r="D72" s="56"/>
@@ -5245,14 +5259,14 @@
       <c r="G72" s="56"/>
       <c r="H72" s="56"/>
       <c r="I72" s="57"/>
-      <c r="J72" s="89"/>
+      <c r="J72" s="82"/>
     </row>
     <row r="73" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="89"/>
-      <c r="B73" s="111">
+      <c r="A73" s="82"/>
+      <c r="B73" s="90">
         <v>67</v>
       </c>
-      <c r="C73" s="124" t="s">
+      <c r="C73" s="100" t="s">
         <v>164</v>
       </c>
       <c r="D73" s="56"/>
@@ -5261,14 +5275,14 @@
       <c r="G73" s="56"/>
       <c r="H73" s="56"/>
       <c r="I73" s="57"/>
-      <c r="J73" s="89"/>
+      <c r="J73" s="82"/>
     </row>
     <row r="74" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="89"/>
-      <c r="B74" s="113">
+      <c r="A74" s="82"/>
+      <c r="B74" s="92">
         <v>68</v>
       </c>
-      <c r="C74" s="124" t="s">
+      <c r="C74" s="100" t="s">
         <v>198</v>
       </c>
       <c r="D74" s="56"/>
@@ -5277,14 +5291,14 @@
       <c r="G74" s="56"/>
       <c r="H74" s="56"/>
       <c r="I74" s="57"/>
-      <c r="J74" s="89"/>
+      <c r="J74" s="82"/>
     </row>
     <row r="75" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="89"/>
-      <c r="B75" s="111">
+      <c r="A75" s="82"/>
+      <c r="B75" s="90">
         <v>69</v>
       </c>
-      <c r="C75" s="124" t="s">
+      <c r="C75" s="100" t="s">
         <v>165</v>
       </c>
       <c r="D75" s="56"/>
@@ -5293,14 +5307,14 @@
       <c r="G75" s="56"/>
       <c r="H75" s="56"/>
       <c r="I75" s="57"/>
-      <c r="J75" s="89"/>
+      <c r="J75" s="82"/>
     </row>
     <row r="76" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="89"/>
-      <c r="B76" s="113">
+      <c r="A76" s="82"/>
+      <c r="B76" s="92">
         <v>70</v>
       </c>
-      <c r="C76" s="124" t="s">
+      <c r="C76" s="100" t="s">
         <v>197</v>
       </c>
       <c r="D76" s="56"/>
@@ -5309,14 +5323,14 @@
       <c r="G76" s="56"/>
       <c r="H76" s="56"/>
       <c r="I76" s="57"/>
-      <c r="J76" s="89"/>
+      <c r="J76" s="82"/>
     </row>
     <row r="77" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="89"/>
-      <c r="B77" s="111">
+      <c r="A77" s="82"/>
+      <c r="B77" s="90">
         <v>71</v>
       </c>
-      <c r="C77" s="124" t="s">
+      <c r="C77" s="100" t="s">
         <v>216</v>
       </c>
       <c r="D77" s="56"/>
@@ -5325,14 +5339,14 @@
       <c r="G77" s="56"/>
       <c r="H77" s="56"/>
       <c r="I77" s="57"/>
-      <c r="J77" s="89"/>
+      <c r="J77" s="82"/>
     </row>
     <row r="78" spans="1:10" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="89"/>
-      <c r="B78" s="125">
+      <c r="A78" s="82"/>
+      <c r="B78" s="101">
         <v>72</v>
       </c>
-      <c r="C78" s="126" t="s">
+      <c r="C78" s="102" t="s">
         <v>193</v>
       </c>
       <c r="D78" s="76"/>
@@ -5341,19 +5355,21 @@
       <c r="G78" s="76"/>
       <c r="H78" s="76"/>
       <c r="I78" s="77"/>
-      <c r="J78" s="89"/>
+      <c r="J78" s="82"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A79" s="89"/>
-      <c r="B79" s="90"/>
-      <c r="C79" s="89"/>
-      <c r="D79" s="89"/>
-      <c r="E79" s="89"/>
-      <c r="F79" s="89"/>
-      <c r="G79" s="89"/>
-      <c r="H79" s="89"/>
-      <c r="I79" s="89"/>
-      <c r="J79" s="89"/>
+      <c r="A79" s="82"/>
+      <c r="B79" s="83"/>
+      <c r="C79" s="82"/>
+      <c r="D79" s="82"/>
+      <c r="E79" s="82"/>
+      <c r="F79" s="82"/>
+      <c r="G79" s="82"/>
+      <c r="H79" s="82"/>
+      <c r="I79" s="82"/>
+      <c r="J79" s="129" t="s">
+        <v>217</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -5374,13 +5390,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:S53"/>
+  <dimension ref="B1:T54"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="8" ySplit="3" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="3" topLeftCell="I46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="T3" sqref="T3"/>
+      <selection pane="bottomRight" activeCell="T54" sqref="T54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5410,44 +5426,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" s="1" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="82" t="s">
+      <c r="B1" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="122"/>
+      <c r="J1" s="122"/>
+      <c r="K1" s="122"/>
+      <c r="L1" s="122"/>
+      <c r="M1" s="122"/>
+      <c r="N1" s="122"/>
+      <c r="O1" s="122"/>
+      <c r="P1" s="122"/>
+      <c r="Q1" s="122"/>
+      <c r="R1" s="122"/>
+      <c r="S1" s="122"/>
     </row>
     <row r="2" spans="2:19" s="2" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="125" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="83" t="s">
+      <c r="C2" s="123" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="87" t="s">
+      <c r="D2" s="127" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="87" t="s">
+      <c r="E2" s="127" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="87" t="s">
+      <c r="F2" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="87" t="s">
+      <c r="G2" s="127" t="s">
         <v>23</v>
       </c>
       <c r="H2" s="29" t="s">
@@ -5488,12 +5504,12 @@
       </c>
     </row>
     <row r="3" spans="2:19" s="26" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="86"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
+      <c r="B3" s="126"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="128"/>
+      <c r="G3" s="128"/>
       <c r="H3" s="24" t="s">
         <v>155</v>
       </c>
@@ -7271,7 +7287,7 @@
       <c r="R48" s="16"/>
       <c r="S48" s="23"/>
     </row>
-    <row r="49" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B49" s="31">
         <v>46</v>
       </c>
@@ -7309,7 +7325,7 @@
       <c r="R49" s="16"/>
       <c r="S49" s="23"/>
     </row>
-    <row r="50" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B50" s="31">
         <v>47</v>
       </c>
@@ -7347,7 +7363,7 @@
       <c r="R50" s="16"/>
       <c r="S50" s="23"/>
     </row>
-    <row r="51" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B51" s="31">
         <v>48</v>
       </c>
@@ -7385,7 +7401,7 @@
       <c r="R51" s="16"/>
       <c r="S51" s="23"/>
     </row>
-    <row r="52" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B52" s="31">
         <v>49</v>
       </c>
@@ -7423,7 +7439,7 @@
       <c r="R52" s="16"/>
       <c r="S52" s="23"/>
     </row>
-    <row r="53" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B53" s="31">
         <v>50</v>
       </c>
@@ -7460,6 +7476,11 @@
       <c r="Q53" s="23"/>
       <c r="R53" s="16"/>
       <c r="S53" s="23"/>
+    </row>
+    <row r="54" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="T54" s="3" t="s">
+        <v>217</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -8358,13 +8379,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:B28"/>
+  <dimension ref="B1:C29"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomRight" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8444,64 +8465,69 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="38" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="37" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B19" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B20" s="37" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="37" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="38" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="38" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="25" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B25" s="37" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="2:2" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="37" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="2:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="37" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="2:2" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="37" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C29" s="33" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>